<commit_message>
Feature CSV file write is completed & Checked.
</commit_message>
<xml_diff>
--- a/DataFiles/RawSignals.xlsx
+++ b/DataFiles/RawSignals.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Charitha" sheetId="3" r:id="rId1"/>
@@ -339,7 +339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AC1" sqref="AC1:AC1048576"/>
     </sheetView>
   </sheetViews>
@@ -20352,8 +20352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH231"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
+      <selection activeCell="A190" sqref="A190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34628,6 +34628,9 @@
       <c r="G138">
         <v>15844</v>
       </c>
+      <c r="H138">
+        <v>15847</v>
+      </c>
       <c r="I138">
         <v>15842</v>
       </c>
@@ -34729,6 +34732,9 @@
       <c r="G139">
         <v>15843</v>
       </c>
+      <c r="H139">
+        <v>15847</v>
+      </c>
       <c r="I139">
         <v>15844</v>
       </c>
@@ -34830,6 +34836,9 @@
       <c r="G140">
         <v>15843</v>
       </c>
+      <c r="H140">
+        <v>15847</v>
+      </c>
       <c r="I140">
         <v>15846</v>
       </c>
@@ -34931,6 +34940,9 @@
       <c r="G141">
         <v>15844</v>
       </c>
+      <c r="H141">
+        <v>15847</v>
+      </c>
       <c r="I141">
         <v>15843</v>
       </c>
@@ -35032,6 +35044,9 @@
       <c r="G142">
         <v>15843</v>
       </c>
+      <c r="H142">
+        <v>15847</v>
+      </c>
       <c r="I142">
         <v>15843</v>
       </c>
@@ -35133,6 +35148,9 @@
       <c r="G143">
         <v>15843</v>
       </c>
+      <c r="H143">
+        <v>15847</v>
+      </c>
       <c r="I143">
         <v>15843</v>
       </c>
@@ -35234,6 +35252,9 @@
       <c r="G144">
         <v>15843</v>
       </c>
+      <c r="H144">
+        <v>15847</v>
+      </c>
       <c r="I144">
         <v>15843</v>
       </c>
@@ -35335,6 +35356,9 @@
       <c r="G145">
         <v>15844</v>
       </c>
+      <c r="H145">
+        <v>15847</v>
+      </c>
       <c r="I145">
         <v>15844</v>
       </c>
@@ -35436,6 +35460,9 @@
       <c r="G146">
         <v>15844</v>
       </c>
+      <c r="H146">
+        <v>15847</v>
+      </c>
       <c r="I146">
         <v>15844</v>
       </c>
@@ -35537,6 +35564,9 @@
       <c r="G147">
         <v>15843</v>
       </c>
+      <c r="H147">
+        <v>15847</v>
+      </c>
       <c r="I147">
         <v>15844</v>
       </c>
@@ -35637,6 +35667,9 @@
       </c>
       <c r="G148">
         <v>15843</v>
+      </c>
+      <c r="H148">
+        <v>15847</v>
       </c>
       <c r="I148">
         <v>15843</v>
@@ -35739,6 +35772,9 @@
       <c r="G149">
         <v>15844</v>
       </c>
+      <c r="H149">
+        <v>15847</v>
+      </c>
       <c r="I149">
         <v>15843</v>
       </c>
@@ -35840,6 +35876,9 @@
       <c r="G150">
         <v>15845</v>
       </c>
+      <c r="H150">
+        <v>15847</v>
+      </c>
       <c r="I150">
         <v>15845</v>
       </c>
@@ -35941,6 +35980,9 @@
       <c r="G151">
         <v>15845</v>
       </c>
+      <c r="H151">
+        <v>15847</v>
+      </c>
       <c r="I151">
         <v>15844</v>
       </c>
@@ -36042,6 +36084,9 @@
       <c r="G152">
         <v>15845</v>
       </c>
+      <c r="H152">
+        <v>15847</v>
+      </c>
       <c r="I152">
         <v>15843</v>
       </c>
@@ -36143,6 +36188,9 @@
       <c r="G153">
         <v>15843</v>
       </c>
+      <c r="H153">
+        <v>15847</v>
+      </c>
       <c r="I153">
         <v>15843</v>
       </c>
@@ -36244,6 +36292,9 @@
       <c r="G154">
         <v>15844</v>
       </c>
+      <c r="H154">
+        <v>15847</v>
+      </c>
       <c r="I154">
         <v>15844</v>
       </c>
@@ -36345,6 +36396,9 @@
       <c r="G155">
         <v>15844</v>
       </c>
+      <c r="H155">
+        <v>15847</v>
+      </c>
       <c r="I155">
         <v>15844</v>
       </c>
@@ -36446,6 +36500,9 @@
       <c r="G156">
         <v>15844</v>
       </c>
+      <c r="H156">
+        <v>15847</v>
+      </c>
       <c r="I156">
         <v>15845</v>
       </c>
@@ -36547,6 +36604,9 @@
       <c r="G157">
         <v>15844</v>
       </c>
+      <c r="H157">
+        <v>15847</v>
+      </c>
       <c r="I157">
         <v>15844</v>
       </c>
@@ -36648,6 +36708,9 @@
       <c r="G158">
         <v>15844</v>
       </c>
+      <c r="H158">
+        <v>15847</v>
+      </c>
       <c r="I158">
         <v>15844</v>
       </c>
@@ -36749,6 +36812,9 @@
       <c r="G159">
         <v>15843</v>
       </c>
+      <c r="H159">
+        <v>15847</v>
+      </c>
       <c r="I159">
         <v>15843</v>
       </c>
@@ -36850,6 +36916,9 @@
       <c r="G160">
         <v>15843</v>
       </c>
+      <c r="H160">
+        <v>15847</v>
+      </c>
       <c r="I160">
         <v>15845</v>
       </c>
@@ -36951,6 +37020,9 @@
       <c r="G161">
         <v>15844</v>
       </c>
+      <c r="H161">
+        <v>15847</v>
+      </c>
       <c r="I161">
         <v>15844</v>
       </c>
@@ -37052,6 +37124,9 @@
       <c r="G162">
         <v>15844</v>
       </c>
+      <c r="H162">
+        <v>15847</v>
+      </c>
       <c r="I162">
         <v>15845</v>
       </c>
@@ -37153,6 +37228,9 @@
       <c r="G163">
         <v>15845</v>
       </c>
+      <c r="H163">
+        <v>15847</v>
+      </c>
       <c r="I163">
         <v>15844</v>
       </c>
@@ -37198,6 +37276,9 @@
       <c r="W163">
         <v>15842</v>
       </c>
+      <c r="X163">
+        <v>15844</v>
+      </c>
       <c r="Y163">
         <v>15844</v>
       </c>
@@ -37251,6 +37332,9 @@
       <c r="G164">
         <v>15844</v>
       </c>
+      <c r="H164">
+        <v>15847</v>
+      </c>
       <c r="I164">
         <v>15844</v>
       </c>
@@ -37296,6 +37380,9 @@
       <c r="W164">
         <v>15848</v>
       </c>
+      <c r="X164">
+        <v>15844</v>
+      </c>
       <c r="Y164">
         <v>15843</v>
       </c>
@@ -37349,6 +37436,9 @@
       <c r="G165">
         <v>15844</v>
       </c>
+      <c r="H165">
+        <v>15847</v>
+      </c>
       <c r="I165">
         <v>15843</v>
       </c>
@@ -37394,6 +37484,9 @@
       <c r="W165">
         <v>15843</v>
       </c>
+      <c r="X165">
+        <v>15844</v>
+      </c>
       <c r="Y165">
         <v>15844</v>
       </c>
@@ -37447,6 +37540,9 @@
       <c r="G166">
         <v>15845</v>
       </c>
+      <c r="H166">
+        <v>15847</v>
+      </c>
       <c r="I166">
         <v>15845</v>
       </c>
@@ -37492,6 +37588,9 @@
       <c r="W166">
         <v>15846</v>
       </c>
+      <c r="X166">
+        <v>15844</v>
+      </c>
       <c r="Y166">
         <v>15844</v>
       </c>
@@ -37524,6 +37623,9 @@
       </c>
     </row>
     <row r="167" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>15844</v>
+      </c>
       <c r="B167">
         <v>15846</v>
       </c>
@@ -37541,6 +37643,9 @@
       </c>
       <c r="G167">
         <v>15844</v>
+      </c>
+      <c r="H167">
+        <v>15847</v>
       </c>
       <c r="I167">
         <v>15844</v>
@@ -37587,6 +37692,9 @@
       <c r="W167">
         <v>15842</v>
       </c>
+      <c r="X167">
+        <v>15844</v>
+      </c>
       <c r="Y167">
         <v>15845</v>
       </c>
@@ -37619,6 +37727,9 @@
       </c>
     </row>
     <row r="168" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>15844</v>
+      </c>
       <c r="B168">
         <v>15844</v>
       </c>
@@ -37636,6 +37747,9 @@
       </c>
       <c r="G168">
         <v>15845</v>
+      </c>
+      <c r="H168">
+        <v>15847</v>
       </c>
       <c r="I168">
         <v>15844</v>
@@ -37682,6 +37796,9 @@
       <c r="W168">
         <v>15844</v>
       </c>
+      <c r="X168">
+        <v>15844</v>
+      </c>
       <c r="Y168">
         <v>15844</v>
       </c>
@@ -37714,6 +37831,9 @@
       </c>
     </row>
     <row r="169" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>15844</v>
+      </c>
       <c r="B169">
         <v>15842</v>
       </c>
@@ -37731,6 +37851,9 @@
       </c>
       <c r="G169">
         <v>15844</v>
+      </c>
+      <c r="H169">
+        <v>15847</v>
       </c>
       <c r="I169">
         <v>15844</v>
@@ -37777,6 +37900,9 @@
       <c r="W169">
         <v>15845</v>
       </c>
+      <c r="X169">
+        <v>15844</v>
+      </c>
       <c r="Y169">
         <v>15843</v>
       </c>
@@ -37809,6 +37935,9 @@
       </c>
     </row>
     <row r="170" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>15844</v>
+      </c>
       <c r="B170">
         <v>15844</v>
       </c>
@@ -37826,6 +37955,9 @@
       </c>
       <c r="G170">
         <v>15844</v>
+      </c>
+      <c r="H170">
+        <v>15847</v>
       </c>
       <c r="I170">
         <v>15845</v>
@@ -37872,6 +38004,9 @@
       <c r="W170">
         <v>15845</v>
       </c>
+      <c r="X170">
+        <v>15844</v>
+      </c>
       <c r="Y170">
         <v>15844</v>
       </c>
@@ -37904,6 +38039,9 @@
       </c>
     </row>
     <row r="171" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>15844</v>
+      </c>
       <c r="B171">
         <v>15845</v>
       </c>
@@ -37921,6 +38059,9 @@
       </c>
       <c r="G171">
         <v>15844</v>
+      </c>
+      <c r="H171">
+        <v>15847</v>
       </c>
       <c r="I171">
         <v>15844</v>
@@ -37967,6 +38108,12 @@
       <c r="W171">
         <v>15843</v>
       </c>
+      <c r="X171">
+        <v>15844</v>
+      </c>
+      <c r="Y171">
+        <v>15844</v>
+      </c>
       <c r="Z171">
         <v>15844</v>
       </c>
@@ -37996,6 +38143,9 @@
       </c>
     </row>
     <row r="172" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>15844</v>
+      </c>
       <c r="B172">
         <v>15844</v>
       </c>
@@ -38014,6 +38164,9 @@
       <c r="G172">
         <v>15844</v>
       </c>
+      <c r="H172">
+        <v>15847</v>
+      </c>
       <c r="I172">
         <v>15844</v>
       </c>
@@ -38058,6 +38211,12 @@
       </c>
       <c r="W172">
         <v>15845</v>
+      </c>
+      <c r="X172">
+        <v>15844</v>
+      </c>
+      <c r="Y172">
+        <v>15844</v>
       </c>
       <c r="Z172">
         <v>15844</v>
@@ -38088,6 +38247,9 @@
       </c>
     </row>
     <row r="173" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>15844</v>
+      </c>
       <c r="B173">
         <v>15844</v>
       </c>
@@ -38106,6 +38268,9 @@
       <c r="G173">
         <v>15844</v>
       </c>
+      <c r="H173">
+        <v>15847</v>
+      </c>
       <c r="I173">
         <v>15845</v>
       </c>
@@ -38151,6 +38316,12 @@
       <c r="W173">
         <v>15843</v>
       </c>
+      <c r="X173">
+        <v>15844</v>
+      </c>
+      <c r="Y173">
+        <v>15844</v>
+      </c>
       <c r="Z173">
         <v>15844</v>
       </c>
@@ -38180,6 +38351,9 @@
       </c>
     </row>
     <row r="174" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>15844</v>
+      </c>
       <c r="B174">
         <v>15845</v>
       </c>
@@ -38198,6 +38372,9 @@
       <c r="G174">
         <v>15844</v>
       </c>
+      <c r="H174">
+        <v>15847</v>
+      </c>
       <c r="I174">
         <v>15844</v>
       </c>
@@ -38241,6 +38418,12 @@
         <v>15844</v>
       </c>
       <c r="W174">
+        <v>15844</v>
+      </c>
+      <c r="X174">
+        <v>15844</v>
+      </c>
+      <c r="Y174">
         <v>15844</v>
       </c>
       <c r="Z174">
@@ -38272,6 +38455,9 @@
       </c>
     </row>
     <row r="175" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>15844</v>
+      </c>
       <c r="B175">
         <v>15845</v>
       </c>
@@ -38290,6 +38476,9 @@
       <c r="G175">
         <v>15844</v>
       </c>
+      <c r="H175">
+        <v>15847</v>
+      </c>
       <c r="I175">
         <v>15844</v>
       </c>
@@ -38335,6 +38524,12 @@
       <c r="W175">
         <v>15845</v>
       </c>
+      <c r="X175">
+        <v>15844</v>
+      </c>
+      <c r="Y175">
+        <v>15844</v>
+      </c>
       <c r="Z175">
         <v>15843</v>
       </c>
@@ -38364,6 +38559,9 @@
       </c>
     </row>
     <row r="176" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>15844</v>
+      </c>
       <c r="B176">
         <v>15843</v>
       </c>
@@ -38382,6 +38580,9 @@
       <c r="G176">
         <v>15844</v>
       </c>
+      <c r="H176">
+        <v>15847</v>
+      </c>
       <c r="I176">
         <v>15844</v>
       </c>
@@ -38406,6 +38607,9 @@
       <c r="P176">
         <v>15844</v>
       </c>
+      <c r="Q176">
+        <v>15843</v>
+      </c>
       <c r="R176">
         <v>15844</v>
       </c>
@@ -38424,6 +38628,12 @@
       <c r="W176">
         <v>15844</v>
       </c>
+      <c r="X176">
+        <v>15844</v>
+      </c>
+      <c r="Y176">
+        <v>15844</v>
+      </c>
       <c r="Z176">
         <v>15843</v>
       </c>
@@ -38452,7 +38662,10 @@
         <v>15845</v>
       </c>
     </row>
-    <row r="177" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>15844</v>
+      </c>
       <c r="B177">
         <v>15847</v>
       </c>
@@ -38471,6 +38684,9 @@
       <c r="G177">
         <v>15844</v>
       </c>
+      <c r="H177">
+        <v>15847</v>
+      </c>
       <c r="I177">
         <v>15844</v>
       </c>
@@ -38495,6 +38711,9 @@
       <c r="P177">
         <v>15844</v>
       </c>
+      <c r="Q177">
+        <v>15843</v>
+      </c>
       <c r="R177">
         <v>15844</v>
       </c>
@@ -38513,6 +38732,12 @@
       <c r="W177">
         <v>15843</v>
       </c>
+      <c r="X177">
+        <v>15844</v>
+      </c>
+      <c r="Y177">
+        <v>15844</v>
+      </c>
       <c r="Z177">
         <v>15844</v>
       </c>
@@ -38541,7 +38766,10 @@
         <v>15845</v>
       </c>
     </row>
-    <row r="178" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>15844</v>
+      </c>
       <c r="B178">
         <v>15846</v>
       </c>
@@ -38560,6 +38788,9 @@
       <c r="G178">
         <v>15844</v>
       </c>
+      <c r="H178">
+        <v>15847</v>
+      </c>
       <c r="I178">
         <v>15844</v>
       </c>
@@ -38581,6 +38812,12 @@
       <c r="O178">
         <v>15843</v>
       </c>
+      <c r="P178">
+        <v>15844</v>
+      </c>
+      <c r="Q178">
+        <v>15843</v>
+      </c>
       <c r="R178">
         <v>15843</v>
       </c>
@@ -38599,6 +38836,12 @@
       <c r="W178">
         <v>15844</v>
       </c>
+      <c r="X178">
+        <v>15844</v>
+      </c>
+      <c r="Y178">
+        <v>15844</v>
+      </c>
       <c r="Z178">
         <v>15843</v>
       </c>
@@ -38627,7 +38870,10 @@
         <v>15843</v>
       </c>
     </row>
-    <row r="179" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>15844</v>
+      </c>
       <c r="B179">
         <v>15847</v>
       </c>
@@ -38646,6 +38892,9 @@
       <c r="G179">
         <v>15844</v>
       </c>
+      <c r="H179">
+        <v>15847</v>
+      </c>
       <c r="I179">
         <v>15844</v>
       </c>
@@ -38667,6 +38916,12 @@
       <c r="O179">
         <v>15844</v>
       </c>
+      <c r="P179">
+        <v>15844</v>
+      </c>
+      <c r="Q179">
+        <v>15843</v>
+      </c>
       <c r="R179">
         <v>15843</v>
       </c>
@@ -38682,6 +38937,15 @@
       <c r="V179">
         <v>15844</v>
       </c>
+      <c r="W179">
+        <v>15844</v>
+      </c>
+      <c r="X179">
+        <v>15844</v>
+      </c>
+      <c r="Y179">
+        <v>15844</v>
+      </c>
       <c r="Z179">
         <v>15844</v>
       </c>
@@ -38710,7 +38974,10 @@
         <v>15844</v>
       </c>
     </row>
-    <row r="180" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>15844</v>
+      </c>
       <c r="B180">
         <v>15843</v>
       </c>
@@ -38728,6 +38995,9 @@
       </c>
       <c r="G180">
         <v>15845</v>
+      </c>
+      <c r="H180">
+        <v>15847</v>
       </c>
       <c r="I180">
         <v>15844</v>
@@ -38750,6 +39020,12 @@
       <c r="O180">
         <v>15844</v>
       </c>
+      <c r="P180">
+        <v>15844</v>
+      </c>
+      <c r="Q180">
+        <v>15843</v>
+      </c>
       <c r="R180">
         <v>15842</v>
       </c>
@@ -38765,6 +39041,15 @@
       <c r="V180">
         <v>15845</v>
       </c>
+      <c r="W180">
+        <v>15844</v>
+      </c>
+      <c r="X180">
+        <v>15844</v>
+      </c>
+      <c r="Y180">
+        <v>15844</v>
+      </c>
       <c r="Z180">
         <v>15843</v>
       </c>
@@ -38793,7 +39078,10 @@
         <v>15843</v>
       </c>
     </row>
-    <row r="181" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>15844</v>
+      </c>
       <c r="B181">
         <v>15844</v>
       </c>
@@ -38811,6 +39099,9 @@
       </c>
       <c r="G181">
         <v>15844</v>
+      </c>
+      <c r="H181">
+        <v>15847</v>
       </c>
       <c r="I181">
         <v>15844</v>
@@ -38833,6 +39124,12 @@
       <c r="O181">
         <v>15844</v>
       </c>
+      <c r="P181">
+        <v>15844</v>
+      </c>
+      <c r="Q181">
+        <v>15843</v>
+      </c>
       <c r="R181">
         <v>15848</v>
       </c>
@@ -38848,6 +39145,15 @@
       <c r="V181">
         <v>15844</v>
       </c>
+      <c r="W181">
+        <v>15844</v>
+      </c>
+      <c r="X181">
+        <v>15844</v>
+      </c>
+      <c r="Y181">
+        <v>15844</v>
+      </c>
       <c r="Z181">
         <v>15844</v>
       </c>
@@ -38866,6 +39172,9 @@
       <c r="AE181">
         <v>15845</v>
       </c>
+      <c r="AF181">
+        <v>15843</v>
+      </c>
       <c r="AG181">
         <v>15843</v>
       </c>
@@ -38873,7 +39182,10 @@
         <v>15842</v>
       </c>
     </row>
-    <row r="182" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>15844</v>
+      </c>
       <c r="B182">
         <v>15845</v>
       </c>
@@ -38892,6 +39204,9 @@
       <c r="G182">
         <v>15844</v>
       </c>
+      <c r="H182">
+        <v>15847</v>
+      </c>
       <c r="I182">
         <v>15844</v>
       </c>
@@ -38912,6 +39227,12 @@
       </c>
       <c r="O182">
         <v>15845</v>
+      </c>
+      <c r="P182">
+        <v>15844</v>
+      </c>
+      <c r="Q182">
+        <v>15843</v>
       </c>
       <c r="R182">
         <v>15836</v>
@@ -38928,6 +39249,15 @@
       <c r="V182">
         <v>15844</v>
       </c>
+      <c r="W182">
+        <v>15844</v>
+      </c>
+      <c r="X182">
+        <v>15844</v>
+      </c>
+      <c r="Y182">
+        <v>15844</v>
+      </c>
       <c r="Z182">
         <v>15843</v>
       </c>
@@ -38946,6 +39276,9 @@
       <c r="AE182">
         <v>15844</v>
       </c>
+      <c r="AF182">
+        <v>15843</v>
+      </c>
       <c r="AG182">
         <v>15844</v>
       </c>
@@ -38953,7 +39286,10 @@
         <v>15844</v>
       </c>
     </row>
-    <row r="183" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>15844</v>
+      </c>
       <c r="B183">
         <v>15843</v>
       </c>
@@ -38971,6 +39307,9 @@
       </c>
       <c r="G183">
         <v>15844</v>
+      </c>
+      <c r="H183">
+        <v>15847</v>
       </c>
       <c r="I183">
         <v>15844</v>
@@ -38993,6 +39332,12 @@
       <c r="O183">
         <v>15843</v>
       </c>
+      <c r="P183">
+        <v>15844</v>
+      </c>
+      <c r="Q183">
+        <v>15843</v>
+      </c>
       <c r="R183">
         <v>15839</v>
       </c>
@@ -39008,6 +39353,15 @@
       <c r="V183">
         <v>15843</v>
       </c>
+      <c r="W183">
+        <v>15844</v>
+      </c>
+      <c r="X183">
+        <v>15844</v>
+      </c>
+      <c r="Y183">
+        <v>15844</v>
+      </c>
       <c r="Z183">
         <v>15843</v>
       </c>
@@ -39026,6 +39380,9 @@
       <c r="AE183">
         <v>15844</v>
       </c>
+      <c r="AF183">
+        <v>15843</v>
+      </c>
       <c r="AG183">
         <v>15844</v>
       </c>
@@ -39033,7 +39390,10 @@
         <v>15843</v>
       </c>
     </row>
-    <row r="184" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>15844</v>
+      </c>
       <c r="B184">
         <v>15845</v>
       </c>
@@ -39052,6 +39412,9 @@
       <c r="G184">
         <v>15844</v>
       </c>
+      <c r="H184">
+        <v>15847</v>
+      </c>
       <c r="I184">
         <v>15844</v>
       </c>
@@ -39073,6 +39436,12 @@
       <c r="O184">
         <v>15844</v>
       </c>
+      <c r="P184">
+        <v>15844</v>
+      </c>
+      <c r="Q184">
+        <v>15843</v>
+      </c>
       <c r="R184">
         <v>15846</v>
       </c>
@@ -39088,6 +39457,15 @@
       <c r="V184">
         <v>15845</v>
       </c>
+      <c r="W184">
+        <v>15844</v>
+      </c>
+      <c r="X184">
+        <v>15844</v>
+      </c>
+      <c r="Y184">
+        <v>15844</v>
+      </c>
       <c r="Z184">
         <v>15844</v>
       </c>
@@ -39106,6 +39484,9 @@
       <c r="AE184">
         <v>15843</v>
       </c>
+      <c r="AF184">
+        <v>15843</v>
+      </c>
       <c r="AG184">
         <v>15845</v>
       </c>
@@ -39113,7 +39494,10 @@
         <v>15843</v>
       </c>
     </row>
-    <row r="185" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>15844</v>
+      </c>
       <c r="B185">
         <v>15844</v>
       </c>
@@ -39132,6 +39516,9 @@
       <c r="G185">
         <v>15844</v>
       </c>
+      <c r="H185">
+        <v>15847</v>
+      </c>
       <c r="I185">
         <v>15844</v>
       </c>
@@ -39153,6 +39540,12 @@
       <c r="O185">
         <v>15844</v>
       </c>
+      <c r="P185">
+        <v>15844</v>
+      </c>
+      <c r="Q185">
+        <v>15843</v>
+      </c>
       <c r="R185">
         <v>15842</v>
       </c>
@@ -39168,6 +39561,15 @@
       <c r="V185">
         <v>15842</v>
       </c>
+      <c r="W185">
+        <v>15844</v>
+      </c>
+      <c r="X185">
+        <v>15844</v>
+      </c>
+      <c r="Y185">
+        <v>15844</v>
+      </c>
       <c r="Z185">
         <v>15844</v>
       </c>
@@ -39186,6 +39588,9 @@
       <c r="AE185">
         <v>15844</v>
       </c>
+      <c r="AF185">
+        <v>15843</v>
+      </c>
       <c r="AG185">
         <v>15844</v>
       </c>
@@ -39193,7 +39598,10 @@
         <v>15843</v>
       </c>
     </row>
-    <row r="186" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>15844</v>
+      </c>
       <c r="B186">
         <v>15843</v>
       </c>
@@ -39212,9 +39620,15 @@
       <c r="G186">
         <v>15844</v>
       </c>
+      <c r="H186">
+        <v>15847</v>
+      </c>
       <c r="I186">
         <v>15844</v>
       </c>
+      <c r="J186">
+        <v>15844</v>
+      </c>
       <c r="K186">
         <v>15843</v>
       </c>
@@ -39229,6 +39643,12 @@
       </c>
       <c r="O186">
         <v>15844</v>
+      </c>
+      <c r="P186">
+        <v>15844</v>
+      </c>
+      <c r="Q186">
+        <v>15843</v>
       </c>
       <c r="R186">
         <v>15839</v>
@@ -39245,6 +39665,15 @@
       <c r="V186">
         <v>15844</v>
       </c>
+      <c r="W186">
+        <v>15844</v>
+      </c>
+      <c r="X186">
+        <v>15844</v>
+      </c>
+      <c r="Y186">
+        <v>15844</v>
+      </c>
       <c r="Z186">
         <v>15844</v>
       </c>
@@ -39263,6 +39692,9 @@
       <c r="AE186">
         <v>15844</v>
       </c>
+      <c r="AF186">
+        <v>15843</v>
+      </c>
       <c r="AG186">
         <v>15844</v>
       </c>
@@ -39270,7 +39702,10 @@
         <v>15843</v>
       </c>
     </row>
-    <row r="187" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>15844</v>
+      </c>
       <c r="B187">
         <v>15844</v>
       </c>
@@ -39289,9 +39724,15 @@
       <c r="G187">
         <v>15844</v>
       </c>
+      <c r="H187">
+        <v>15847</v>
+      </c>
       <c r="I187">
         <v>15844</v>
       </c>
+      <c r="J187">
+        <v>15844</v>
+      </c>
       <c r="K187">
         <v>15843</v>
       </c>
@@ -39307,6 +39748,12 @@
       <c r="O187">
         <v>15845</v>
       </c>
+      <c r="P187">
+        <v>15844</v>
+      </c>
+      <c r="Q187">
+        <v>15843</v>
+      </c>
       <c r="R187">
         <v>15845</v>
       </c>
@@ -39322,6 +39769,15 @@
       <c r="V187">
         <v>15843</v>
       </c>
+      <c r="W187">
+        <v>15844</v>
+      </c>
+      <c r="X187">
+        <v>15844</v>
+      </c>
+      <c r="Y187">
+        <v>15844</v>
+      </c>
       <c r="Z187">
         <v>15844</v>
       </c>
@@ -39340,6 +39796,9 @@
       <c r="AE187">
         <v>15843</v>
       </c>
+      <c r="AF187">
+        <v>15843</v>
+      </c>
       <c r="AG187">
         <v>15843</v>
       </c>
@@ -39347,7 +39806,10 @@
         <v>15844</v>
       </c>
     </row>
-    <row r="188" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>15844</v>
+      </c>
       <c r="B188">
         <v>15843</v>
       </c>
@@ -39366,6 +39828,15 @@
       <c r="G188">
         <v>15844</v>
       </c>
+      <c r="H188">
+        <v>15847</v>
+      </c>
+      <c r="I188">
+        <v>15844</v>
+      </c>
+      <c r="J188">
+        <v>15844</v>
+      </c>
       <c r="K188">
         <v>15845</v>
       </c>
@@ -39379,6 +39850,12 @@
         <v>15843</v>
       </c>
       <c r="O188">
+        <v>15843</v>
+      </c>
+      <c r="P188">
+        <v>15844</v>
+      </c>
+      <c r="Q188">
         <v>15843</v>
       </c>
       <c r="R188">
@@ -39396,6 +39873,15 @@
       <c r="V188">
         <v>15845</v>
       </c>
+      <c r="W188">
+        <v>15844</v>
+      </c>
+      <c r="X188">
+        <v>15844</v>
+      </c>
+      <c r="Y188">
+        <v>15844</v>
+      </c>
       <c r="Z188">
         <v>15843</v>
       </c>
@@ -39414,6 +39900,9 @@
       <c r="AE188">
         <v>15843</v>
       </c>
+      <c r="AF188">
+        <v>15843</v>
+      </c>
       <c r="AG188">
         <v>15844</v>
       </c>
@@ -39421,7 +39910,10 @@
         <v>15843</v>
       </c>
     </row>
-    <row r="189" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>15844</v>
+      </c>
       <c r="B189">
         <v>15844</v>
       </c>
@@ -39440,6 +39932,15 @@
       <c r="G189">
         <v>15844</v>
       </c>
+      <c r="H189">
+        <v>15847</v>
+      </c>
+      <c r="I189">
+        <v>15844</v>
+      </c>
+      <c r="J189">
+        <v>15844</v>
+      </c>
       <c r="K189">
         <v>15844</v>
       </c>
@@ -39455,6 +39956,12 @@
       <c r="O189">
         <v>15844</v>
       </c>
+      <c r="P189">
+        <v>15844</v>
+      </c>
+      <c r="Q189">
+        <v>15843</v>
+      </c>
       <c r="R189">
         <v>15842</v>
       </c>
@@ -39465,6 +39972,18 @@
         <v>15844</v>
       </c>
       <c r="U189">
+        <v>15844</v>
+      </c>
+      <c r="V189">
+        <v>15845</v>
+      </c>
+      <c r="W189">
+        <v>15844</v>
+      </c>
+      <c r="X189">
+        <v>15844</v>
+      </c>
+      <c r="Y189">
         <v>15844</v>
       </c>
       <c r="Z189">
@@ -39485,11 +40004,20 @@
       <c r="AE189">
         <v>15843</v>
       </c>
+      <c r="AF189">
+        <v>15843</v>
+      </c>
+      <c r="AG189">
+        <v>15844</v>
+      </c>
       <c r="AH189">
         <v>15844</v>
       </c>
     </row>
-    <row r="190" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>15844</v>
+      </c>
       <c r="B190">
         <v>15844</v>
       </c>
@@ -39508,6 +40036,15 @@
       <c r="G190">
         <v>15844</v>
       </c>
+      <c r="H190">
+        <v>15847</v>
+      </c>
+      <c r="I190">
+        <v>15844</v>
+      </c>
+      <c r="J190">
+        <v>15844</v>
+      </c>
       <c r="K190">
         <v>15843</v>
       </c>
@@ -39523,6 +40060,12 @@
       <c r="O190">
         <v>15844</v>
       </c>
+      <c r="P190">
+        <v>15844</v>
+      </c>
+      <c r="Q190">
+        <v>15843</v>
+      </c>
       <c r="R190">
         <v>15843</v>
       </c>
@@ -39535,9 +40078,24 @@
       <c r="U190">
         <v>15844</v>
       </c>
+      <c r="V190">
+        <v>15845</v>
+      </c>
+      <c r="W190">
+        <v>15844</v>
+      </c>
+      <c r="X190">
+        <v>15844</v>
+      </c>
+      <c r="Y190">
+        <v>15844</v>
+      </c>
       <c r="Z190">
         <v>15843</v>
       </c>
+      <c r="AA190">
+        <v>15843</v>
+      </c>
       <c r="AB190">
         <v>15843</v>
       </c>
@@ -39550,11 +40108,17 @@
       <c r="AE190">
         <v>15844</v>
       </c>
+      <c r="AF190">
+        <v>15843</v>
+      </c>
+      <c r="AG190">
+        <v>15844</v>
+      </c>
       <c r="AH190">
         <v>15842</v>
       </c>
     </row>
-    <row r="191" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B191">
         <v>15845</v>
       </c>
@@ -39573,6 +40137,15 @@
       <c r="G191">
         <v>15844</v>
       </c>
+      <c r="H191">
+        <v>15847</v>
+      </c>
+      <c r="I191">
+        <v>15844</v>
+      </c>
+      <c r="J191">
+        <v>15844</v>
+      </c>
       <c r="K191">
         <v>15843</v>
       </c>
@@ -39588,6 +40161,12 @@
       <c r="O191">
         <v>15845</v>
       </c>
+      <c r="P191">
+        <v>15844</v>
+      </c>
+      <c r="Q191">
+        <v>15843</v>
+      </c>
       <c r="R191">
         <v>15844</v>
       </c>
@@ -39600,8 +40179,23 @@
       <c r="U191">
         <v>15843</v>
       </c>
+      <c r="V191">
+        <v>15845</v>
+      </c>
+      <c r="W191">
+        <v>15844</v>
+      </c>
+      <c r="X191">
+        <v>15844</v>
+      </c>
+      <c r="Y191">
+        <v>15844</v>
+      </c>
       <c r="Z191">
         <v>15844</v>
+      </c>
+      <c r="AA191">
+        <v>15843</v>
       </c>
       <c r="AB191">
         <v>15843</v>
@@ -39615,11 +40209,17 @@
       <c r="AE191">
         <v>15844</v>
       </c>
+      <c r="AF191">
+        <v>15843</v>
+      </c>
+      <c r="AG191">
+        <v>15844</v>
+      </c>
       <c r="AH191">
         <v>15843</v>
       </c>
     </row>
-    <row r="192" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B192">
         <v>15844</v>
       </c>
@@ -39635,6 +40235,15 @@
       <c r="G192">
         <v>15844</v>
       </c>
+      <c r="H192">
+        <v>15847</v>
+      </c>
+      <c r="I192">
+        <v>15844</v>
+      </c>
+      <c r="J192">
+        <v>15844</v>
+      </c>
       <c r="K192">
         <v>15843</v>
       </c>
@@ -39650,6 +40259,12 @@
       <c r="O192">
         <v>15844</v>
       </c>
+      <c r="P192">
+        <v>15844</v>
+      </c>
+      <c r="Q192">
+        <v>15843</v>
+      </c>
       <c r="R192">
         <v>15843</v>
       </c>
@@ -39662,9 +40277,24 @@
       <c r="U192">
         <v>15844</v>
       </c>
+      <c r="V192">
+        <v>15845</v>
+      </c>
+      <c r="W192">
+        <v>15844</v>
+      </c>
+      <c r="X192">
+        <v>15844</v>
+      </c>
+      <c r="Y192">
+        <v>15844</v>
+      </c>
       <c r="Z192">
         <v>15843</v>
       </c>
+      <c r="AA192">
+        <v>15843</v>
+      </c>
       <c r="AB192">
         <v>15843</v>
       </c>
@@ -39676,6 +40306,12 @@
       </c>
       <c r="AE192">
         <v>15845</v>
+      </c>
+      <c r="AF192">
+        <v>15843</v>
+      </c>
+      <c r="AG192">
+        <v>15844</v>
       </c>
       <c r="AH192">
         <v>15845</v>
@@ -39718,9 +40354,15 @@
       <c r="U193">
         <v>15845</v>
       </c>
+      <c r="Y193">
+        <v>15844</v>
+      </c>
       <c r="Z193">
         <v>15844</v>
       </c>
+      <c r="AA193">
+        <v>15843</v>
+      </c>
       <c r="AB193">
         <v>15843</v>
       </c>
@@ -39731,6 +40373,12 @@
         <v>15844</v>
       </c>
       <c r="AE193">
+        <v>15844</v>
+      </c>
+      <c r="AF193">
+        <v>15843</v>
+      </c>
+      <c r="AG193">
         <v>15844</v>
       </c>
       <c r="AH193">
@@ -39777,6 +40425,9 @@
       <c r="Z194">
         <v>15843</v>
       </c>
+      <c r="AA194">
+        <v>15843</v>
+      </c>
       <c r="AB194">
         <v>15844</v>
       </c>
@@ -39787,6 +40438,12 @@
         <v>15843</v>
       </c>
       <c r="AE194">
+        <v>15844</v>
+      </c>
+      <c r="AF194">
+        <v>15843</v>
+      </c>
+      <c r="AG194">
         <v>15844</v>
       </c>
       <c r="AH194">
@@ -39836,6 +40493,12 @@
       <c r="AD195">
         <v>15844</v>
       </c>
+      <c r="AF195">
+        <v>15843</v>
+      </c>
+      <c r="AG195">
+        <v>15844</v>
+      </c>
       <c r="AH195">
         <v>15843</v>
       </c>
@@ -39881,6 +40544,12 @@
         <v>15843</v>
       </c>
       <c r="AD196">
+        <v>15844</v>
+      </c>
+      <c r="AF196">
+        <v>15843</v>
+      </c>
+      <c r="AG196">
         <v>15844</v>
       </c>
       <c r="AH196">

</xml_diff>